<commit_message>
add appropriate spaces to board layout
</commit_message>
<xml_diff>
--- a/Connections for Continuity board.xlsx
+++ b/Connections for Continuity board.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donald.hersam\Documents\Continuity-Checker-Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04E8A36-8A67-4A7D-8FC3-72573B63A9B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BAB0BB-BA0F-43F1-8F66-C12C07E91EE1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{3701C057-4630-41B1-A314-4A62507DF68A}"/>
   </bookViews>
@@ -557,7 +557,7 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="5">
         <v>18</v>
       </c>
       <c r="D2" s="1"/>
@@ -570,7 +570,7 @@
       <c r="B3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="5">
         <v>18</v>
       </c>
       <c r="D3" s="1"/>

</xml_diff>

<commit_message>
routed all connector breakouts
</commit_message>
<xml_diff>
--- a/Connections for Continuity board.xlsx
+++ b/Connections for Continuity board.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donald.hersam\Documents\Continuity-Checker-Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BAB0BB-BA0F-43F1-8F66-C12C07E91EE1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A79C89B-2638-4A96-B9F9-56E42EAF6934}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{3701C057-4630-41B1-A314-4A62507DF68A}"/>
+    <workbookView xWindow="405" yWindow="375" windowWidth="21600" windowHeight="11385" xr2:uid="{3701C057-4630-41B1-A314-4A62507DF68A}"/>
   </bookViews>
   <sheets>
     <sheet name="Connections" sheetId="1" r:id="rId1"/>
@@ -139,7 +139,7 @@
     <t>Test Point</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/RCU-0C/A106145CT-ND/3477802</t>
+    <t>https://www.digikey.com/product-detail/en/keystone-electronics/5029/36-5029CT-ND/5980631</t>
   </si>
 </sst>
 </file>
@@ -171,7 +171,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +181,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -198,7 +204,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -209,6 +215,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -529,7 +538,7 @@
   <dimension ref="A1:E355"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,7 +569,7 @@
       <c r="C2" s="5">
         <v>18</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="6"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -573,7 +582,7 @@
       <c r="C3" s="5">
         <v>18</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="6"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -586,7 +595,7 @@
       <c r="C4" s="5">
         <v>11</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -599,7 +608,7 @@
       <c r="C5" s="5">
         <v>9</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -612,7 +621,7 @@
       <c r="C6" s="5">
         <v>8</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -625,7 +634,7 @@
       <c r="C7" s="5">
         <v>8</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -638,7 +647,7 @@
       <c r="C8" s="5">
         <v>8</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -651,7 +660,7 @@
       <c r="C9" s="5">
         <v>8</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -664,7 +673,7 @@
       <c r="C10" s="5">
         <v>7</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -677,7 +686,7 @@
       <c r="C11" s="5">
         <v>7</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="6"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -690,7 +699,7 @@
       <c r="C12" s="5">
         <v>6</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="6"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -703,7 +712,7 @@
       <c r="C13" s="5">
         <v>6</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="6"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -716,7 +725,7 @@
       <c r="C14" s="5">
         <v>5</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="6"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -3209,7 +3218,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
remove all erc errors
</commit_message>
<xml_diff>
--- a/Connections for Continuity board.xlsx
+++ b/Connections for Continuity board.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donald.hersam\Documents\Continuity-Checker-Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A79C89B-2638-4A96-B9F9-56E42EAF6934}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7D15A2-6819-4BF4-96B3-BACAB8D1928C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="405" yWindow="375" windowWidth="21600" windowHeight="11385" xr2:uid="{3701C057-4630-41B1-A314-4A62507DF68A}"/>
   </bookViews>
@@ -538,7 +538,7 @@
   <dimension ref="A1:E355"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,7 +738,7 @@
       <c r="C15" s="5">
         <v>4</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="6"/>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -751,7 +751,7 @@
       <c r="C16" s="5">
         <v>4</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="6"/>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -764,7 +764,7 @@
       <c r="C17" s="5">
         <v>4</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="6"/>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -777,7 +777,7 @@
       <c r="C18" s="5">
         <v>4</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="6"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -790,7 +790,7 @@
       <c r="C19" s="5">
         <v>4</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19" s="6"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -803,7 +803,7 @@
       <c r="C20" s="5">
         <v>4</v>
       </c>
-      <c r="D20" s="1"/>
+      <c r="D20" s="6"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -816,7 +816,7 @@
       <c r="C21" s="5">
         <v>4</v>
       </c>
-      <c r="D21" s="1"/>
+      <c r="D21" s="6"/>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -829,7 +829,7 @@
       <c r="C22" s="5">
         <v>4</v>
       </c>
-      <c r="D22" s="1"/>
+      <c r="D22" s="6"/>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -842,7 +842,7 @@
       <c r="C23" s="5">
         <v>4</v>
       </c>
-      <c r="D23" s="1"/>
+      <c r="D23" s="6"/>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -855,7 +855,7 @@
       <c r="C24" s="5">
         <v>4</v>
       </c>
-      <c r="D24" s="1"/>
+      <c r="D24" s="6"/>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -868,7 +868,7 @@
       <c r="C25" s="5">
         <v>3</v>
       </c>
-      <c r="D25" s="1"/>
+      <c r="D25" s="6"/>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -881,7 +881,7 @@
       <c r="C26" s="5">
         <v>3</v>
       </c>
-      <c r="D26" s="1"/>
+      <c r="D26" s="6"/>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -894,7 +894,7 @@
       <c r="C27" s="5">
         <v>2</v>
       </c>
-      <c r="D27" s="1"/>
+      <c r="D27" s="6"/>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -907,7 +907,7 @@
       <c r="C28" s="5">
         <v>2</v>
       </c>
-      <c r="D28" s="1"/>
+      <c r="D28" s="6"/>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
configure rats nest in pcb view
</commit_message>
<xml_diff>
--- a/Connections for Continuity board.xlsx
+++ b/Connections for Continuity board.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donald.hersam\Documents\Continuity-Checker-Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7D15A2-6819-4BF4-96B3-BACAB8D1928C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6807AD0E-1BAC-4084-934A-F90BB9EFCCBB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="405" yWindow="375" windowWidth="21600" windowHeight="11385" xr2:uid="{3701C057-4630-41B1-A314-4A62507DF68A}"/>
   </bookViews>
@@ -538,7 +538,7 @@
   <dimension ref="A1:E355"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +567,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="5">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="1"/>
@@ -593,7 +593,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="5">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="1"/>
@@ -606,7 +606,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="1"/>
@@ -619,7 +619,7 @@
         <v>23</v>
       </c>
       <c r="C6" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="1"/>
@@ -671,7 +671,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="1"/>
@@ -926,7 +926,7 @@
       </c>
       <c r="E30" s="1">
         <f>SUM(C2:C28)</f>
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
convert all test points to through hole
</commit_message>
<xml_diff>
--- a/Connections for Continuity board.xlsx
+++ b/Connections for Continuity board.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donald.hersam\Documents\Continuity-Checker-Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DEB744-A9CE-4FC9-B89B-D8FF7CD385E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D969305-5DAB-49E8-B135-F8EA6FE68D6F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="375" windowWidth="21600" windowHeight="11385" xr2:uid="{3701C057-4630-41B1-A314-4A62507DF68A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3701C057-4630-41B1-A314-4A62507DF68A}"/>
   </bookViews>
   <sheets>
     <sheet name="Connections" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Flight Board Programming</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>166-167</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/keystone-electronics/680/36-680-ND/316581</t>
   </si>
 </sst>
 </file>
@@ -627,7 +630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE6FDE56-E9E5-4442-A855-7A091589097C}">
   <dimension ref="A1:E355"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
@@ -3360,10 +3363,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC53649-C4D4-4022-9A33-79B6D6C83122}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3371,7 +3374,7 @@
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -3379,19 +3382,25 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{C09CAFE8-BD72-453A-9725-D304CC0EE1CC}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{3A7A4D00-AFBD-4D58-BB7F-C76AEFD74282}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>